<commit_message>
loading raw csv data
</commit_message>
<xml_diff>
--- a/all_data_clean.xlsx
+++ b/all_data_clean.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arwenn Kummer\Documents\UCT 2024\BIO3018R\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arwenn Kummer\Documents\GIT\Data Management Course 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F94D3F-0BEF-49EC-9FAC-2181070C5D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394BBD42-8210-481B-83D3-2E168F40BFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F967243F-84F5-4B40-83C7-B7BFB31A3C9D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F967243F-84F5-4B40-83C7-B7BFB31A3C9D}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="2" r:id="rId1"/>
@@ -166,9 +166,6 @@
     <t>Timothy Musaya</t>
   </si>
   <si>
-    <t>Slie</t>
-  </si>
-  <si>
     <t>Collectors:</t>
   </si>
   <si>
@@ -196,27 +193,6 @@
     <t>agraulomyrmex.sp</t>
   </si>
   <si>
-    <t>monomorium.1</t>
-  </si>
-  <si>
-    <t>monomorium.2</t>
-  </si>
-  <si>
-    <t>pheidole.aaa</t>
-  </si>
-  <si>
-    <t>pheidole.aba</t>
-  </si>
-  <si>
-    <t>pheidole.aac</t>
-  </si>
-  <si>
-    <t>lepisiota.1</t>
-  </si>
-  <si>
-    <t>lepisiota.2</t>
-  </si>
-  <si>
     <t>pachycondyla.sp</t>
   </si>
   <si>
@@ -224,6 +200,30 @@
   </si>
   <si>
     <t>unknown.sp</t>
+  </si>
+  <si>
+    <t>monomorium.sp1</t>
+  </si>
+  <si>
+    <t>monomorium.sp2</t>
+  </si>
+  <si>
+    <t>lepisiota.sp1</t>
+  </si>
+  <si>
+    <t>lepisiota.sp2</t>
+  </si>
+  <si>
+    <t>pheidole.sp1</t>
+  </si>
+  <si>
+    <t>pheidole.sp2</t>
+  </si>
+  <si>
+    <t>pheidole.sp3</t>
+  </si>
+  <si>
+    <t>Lindiwe Khoza</t>
   </si>
 </sst>
 </file>
@@ -231,7 +231,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-1C09]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1C09]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -268,12 +268,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,7 +594,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,15 +619,15 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2">
         <v>45323</v>
@@ -635,7 +638,7 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="2">
         <v>45324</v>
@@ -647,8 +650,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
+      <c r="A10" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49974ED1-1EFE-4E44-B2D2-193712845F15}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1241,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EC342F-E307-4BC0-B7F5-9237151A3D09}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:O38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,49 +1269,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
+      <c r="N1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
         <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>